<commit_message>
calibration page & time set & elapsed time
calibration page just initialized but not connected to keypad
time set & elapsed time ok
</commit_message>
<xml_diff>
--- a/Src/assets/texts/texts.xlsx
+++ b/Src/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19453" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23890" uniqueCount="310">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -835,6 +835,150 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0     </t>
   </si>
 </sst>
 </file>
@@ -2329,6 +2473,25 @@
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
+      <c r="B12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
       <c r="M12" s="16" t="s">
         <v>27</v>
       </c>
@@ -3482,7 +3645,7 @@
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C68" t="s">
         <v>41</v>
@@ -3499,7 +3662,7 @@
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C69" t="s">
         <v>41</v>
@@ -3516,37 +3679,616 @@
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C70" t="s">
         <v>41</v>
       </c>
       <c r="D70" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E70" t="s">
         <v>46</v>
       </c>
       <c r="F70" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>264</v>
+      </c>
+      <c r="C71" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" t="s">
+        <v>50</v>
+      </c>
+      <c r="E71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F71" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>265</v>
+      </c>
+      <c r="C72" t="s">
+        <v>41</v>
+      </c>
+      <c r="D72" t="s">
+        <v>45</v>
+      </c>
+      <c r="E72" t="s">
+        <v>46</v>
+      </c>
+      <c r="F72" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>266</v>
+      </c>
+      <c r="C73" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" t="s">
+        <v>50</v>
+      </c>
+      <c r="E73" t="s">
+        <v>46</v>
+      </c>
+      <c r="F73" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>267</v>
+      </c>
+      <c r="C74" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" t="s">
+        <v>45</v>
+      </c>
+      <c r="E74" t="s">
+        <v>46</v>
+      </c>
+      <c r="F74" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>268</v>
+      </c>
+      <c r="C75" t="s">
+        <v>41</v>
+      </c>
+      <c r="D75" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" t="s">
+        <v>46</v>
+      </c>
+      <c r="F75" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>269</v>
+      </c>
+      <c r="C76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D76" t="s">
+        <v>45</v>
+      </c>
+      <c r="E76" t="s">
+        <v>46</v>
+      </c>
+      <c r="F76" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>270</v>
+      </c>
+      <c r="C77" t="s">
+        <v>41</v>
+      </c>
+      <c r="D77" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" t="s">
+        <v>46</v>
+      </c>
+      <c r="F77" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>271</v>
+      </c>
+      <c r="C78" t="s">
+        <v>41</v>
+      </c>
+      <c r="D78" t="s">
+        <v>45</v>
+      </c>
+      <c r="E78" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>272</v>
+      </c>
+      <c r="C79" t="s">
+        <v>41</v>
+      </c>
+      <c r="D79" t="s">
+        <v>50</v>
+      </c>
+      <c r="E79" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>273</v>
+      </c>
+      <c r="C80" t="s">
+        <v>41</v>
+      </c>
+      <c r="D80" t="s">
+        <v>45</v>
+      </c>
+      <c r="E80" t="s">
+        <v>46</v>
+      </c>
+      <c r="F80" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>274</v>
+      </c>
+      <c r="C81" t="s">
+        <v>41</v>
+      </c>
+      <c r="D81" t="s">
+        <v>50</v>
+      </c>
+      <c r="E81" t="s">
+        <v>46</v>
+      </c>
+      <c r="F81" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>275</v>
+      </c>
+      <c r="C82" t="s">
+        <v>41</v>
+      </c>
+      <c r="D82" t="s">
+        <v>45</v>
+      </c>
+      <c r="E82" t="s">
+        <v>46</v>
+      </c>
+      <c r="F82" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>276</v>
+      </c>
+      <c r="C83" t="s">
+        <v>41</v>
+      </c>
+      <c r="D83" t="s">
+        <v>50</v>
+      </c>
+      <c r="E83" t="s">
+        <v>46</v>
+      </c>
+      <c r="F83" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>277</v>
+      </c>
+      <c r="C84" t="s">
+        <v>41</v>
+      </c>
+      <c r="D84" t="s">
+        <v>45</v>
+      </c>
+      <c r="E84" t="s">
+        <v>46</v>
+      </c>
+      <c r="F84" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>278</v>
+      </c>
+      <c r="C85" t="s">
+        <v>41</v>
+      </c>
+      <c r="D85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" t="s">
+        <v>46</v>
+      </c>
+      <c r="F85" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="s">
+        <v>279</v>
+      </c>
+      <c r="C86" t="s">
+        <v>41</v>
+      </c>
+      <c r="D86" t="s">
+        <v>45</v>
+      </c>
+      <c r="E86" t="s">
+        <v>46</v>
+      </c>
+      <c r="F86" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C87" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" t="s">
+        <v>50</v>
+      </c>
+      <c r="E87" t="s">
+        <v>46</v>
+      </c>
+      <c r="F87" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
+        <v>281</v>
+      </c>
+      <c r="C88" t="s">
+        <v>41</v>
+      </c>
+      <c r="D88" t="s">
+        <v>45</v>
+      </c>
+      <c r="E88" t="s">
+        <v>46</v>
+      </c>
+      <c r="F88" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="s">
+        <v>282</v>
+      </c>
+      <c r="C89" t="s">
+        <v>41</v>
+      </c>
+      <c r="D89" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" t="s">
+        <v>46</v>
+      </c>
+      <c r="F89" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="s">
+        <v>283</v>
+      </c>
+      <c r="C90" t="s">
+        <v>262</v>
+      </c>
+      <c r="D90" t="s">
+        <v>50</v>
+      </c>
+      <c r="E90" t="s">
+        <v>46</v>
+      </c>
+      <c r="F90" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
+        <v>284</v>
+      </c>
+      <c r="C91" t="s">
+        <v>262</v>
+      </c>
+      <c r="D91" t="s">
+        <v>50</v>
+      </c>
+      <c r="E91" t="s">
+        <v>46</v>
+      </c>
+      <c r="F91" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="s">
+        <v>285</v>
+      </c>
+      <c r="C92" t="s">
+        <v>262</v>
+      </c>
+      <c r="D92" t="s">
+        <v>50</v>
+      </c>
+      <c r="E92" t="s">
+        <v>46</v>
+      </c>
+      <c r="F92" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="s">
+        <v>286</v>
+      </c>
+      <c r="C93" t="s">
+        <v>262</v>
+      </c>
+      <c r="D93" t="s">
+        <v>50</v>
+      </c>
+      <c r="E93" t="s">
+        <v>46</v>
+      </c>
+      <c r="F93" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
+        <v>287</v>
+      </c>
+      <c r="C94" t="s">
+        <v>262</v>
+      </c>
+      <c r="D94" t="s">
+        <v>50</v>
+      </c>
+      <c r="E94" t="s">
+        <v>46</v>
+      </c>
+      <c r="F94" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="s">
+        <v>288</v>
+      </c>
+      <c r="C95" t="s">
+        <v>262</v>
+      </c>
+      <c r="D95" t="s">
+        <v>50</v>
+      </c>
+      <c r="E95" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="s">
+        <v>289</v>
+      </c>
+      <c r="C96" t="s">
+        <v>262</v>
+      </c>
+      <c r="D96" t="s">
+        <v>50</v>
+      </c>
+      <c r="E96" t="s">
+        <v>46</v>
+      </c>
+      <c r="F96" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="s">
+        <v>290</v>
+      </c>
+      <c r="C97" t="s">
+        <v>262</v>
+      </c>
+      <c r="D97" t="s">
+        <v>50</v>
+      </c>
+      <c r="E97" t="s">
+        <v>46</v>
+      </c>
+      <c r="F97" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="s">
+        <v>291</v>
+      </c>
+      <c r="C98" t="s">
+        <v>262</v>
+      </c>
+      <c r="D98" t="s">
+        <v>50</v>
+      </c>
+      <c r="E98" t="s">
+        <v>46</v>
+      </c>
+      <c r="F98" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="s">
+        <v>292</v>
+      </c>
+      <c r="C99" t="s">
+        <v>262</v>
+      </c>
+      <c r="D99" t="s">
+        <v>50</v>
+      </c>
+      <c r="E99" t="s">
+        <v>46</v>
+      </c>
+      <c r="F99" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s">
+        <v>293</v>
+      </c>
+      <c r="C100" t="s">
+        <v>135</v>
+      </c>
+      <c r="D100" t="s">
+        <v>50</v>
+      </c>
+      <c r="E100" t="s">
+        <v>46</v>
+      </c>
+      <c r="F100" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s">
+        <v>304</v>
+      </c>
+      <c r="C101" t="s">
+        <v>74</v>
+      </c>
+      <c r="D101" t="s">
+        <v>45</v>
+      </c>
+      <c r="E101" t="s">
+        <v>46</v>
+      </c>
+      <c r="F101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s">
+        <v>305</v>
+      </c>
+      <c r="C102" t="s">
+        <v>74</v>
+      </c>
+      <c r="D102" t="s">
+        <v>102</v>
+      </c>
+      <c r="E102" t="s">
+        <v>46</v>
+      </c>
+      <c r="F102" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s">
+        <v>306</v>
+      </c>
+      <c r="C103" t="s">
+        <v>74</v>
+      </c>
+      <c r="D103" t="s">
+        <v>45</v>
+      </c>
+      <c r="E103" t="s">
+        <v>46</v>
+      </c>
+      <c r="F103" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s">
+        <v>307</v>
+      </c>
+      <c r="C104" t="s">
+        <v>74</v>
+      </c>
+      <c r="D104" t="s">
+        <v>102</v>
+      </c>
+      <c r="E104" t="s">
+        <v>46</v>
+      </c>
+      <c r="F104" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="s">
+        <v>308</v>
+      </c>
+      <c r="C105" t="s">
+        <v>41</v>
+      </c>
+      <c r="D105" t="s">
+        <v>50</v>
+      </c>
+      <c r="E105" t="s">
+        <v>46</v>
+      </c>
+      <c r="F105" t="s">
+        <v>247</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
calibration page and time modes published
</commit_message>
<xml_diff>
--- a/Src/assets/texts/texts.xlsx
+++ b/Src/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23890" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24541" uniqueCount="312">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -979,6 +979,12 @@
   </si>
   <si>
     <t xml:space="preserve">   0     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop</t>
   </si>
 </sst>
 </file>
@@ -4289,6 +4295,23 @@
         <v>247</v>
       </c>
     </row>
+    <row r="106">
+      <c r="B106" t="s">
+        <v>310</v>
+      </c>
+      <c r="C106" t="s">
+        <v>41</v>
+      </c>
+      <c r="D106" t="s">
+        <v>45</v>
+      </c>
+      <c r="E106" t="s">
+        <v>46</v>
+      </c>
+      <c r="F106" t="s">
+        <v>311</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
time mode & infinite mode
time mode & infinite mode change from auto mode(time set =0 or not) to button mode.
</commit_message>
<xml_diff>
--- a/Src/assets/texts/texts.xlsx
+++ b/Src/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24541" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25198" uniqueCount="314">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -985,6 +985,13 @@
   </si>
   <si>
     <t xml:space="preserve">Stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infinite
+ Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId163</t>
   </si>
 </sst>
 </file>
@@ -2762,7 +2769,7 @@
         <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16">
@@ -4310,6 +4317,23 @@
       </c>
       <c r="F106" t="s">
         <v>311</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="s">
+        <v>313</v>
+      </c>
+      <c r="C107" t="s">
+        <v>41</v>
+      </c>
+      <c r="D107" t="s">
+        <v>45</v>
+      </c>
+      <c r="E107" t="s">
+        <v>46</v>
+      </c>
+      <c r="F107" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>